<commit_message>
learn many courses this weekend
</commit_message>
<xml_diff>
--- a/OS_From_Zero/Doc/4周学RTOS课程初步安排.xlsx
+++ b/OS_From_Zero/Doc/4周学RTOS课程初步安排.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lishutong/Documents/发烧友课程计划/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roy\Desktop\Proj Local\OS_Study\OS_From_Zero\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15900" tabRatio="500"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="25605" windowHeight="15900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -1751,7 +1751,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1776,7 +1776,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1798,6 +1798,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1866,7 +1872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1877,6 +1883,57 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1890,59 +1947,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1953,6 +1962,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2223,22 +2235,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D23"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.875" style="2" customWidth="1"/>
     <col min="4" max="4" width="50" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="28.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2258,576 +2270,604 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="22" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="22"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="3" t="s">
+    <row r="4" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="22"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="3" t="s">
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="22"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="3" t="s">
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="3" t="s">
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="3" t="s">
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="22"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="3" t="s">
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="22"/>
-      <c r="B10" s="14" t="s">
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="22"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="3" t="s">
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="22"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="3" t="s">
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A12" s="8"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="23"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="3" t="s">
+      <c r="F12" s="23"/>
+    </row>
+    <row r="13" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A13" s="9"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F13" s="24"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="12.95" customHeight="1">
       <c r="A15" s="12"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="4" t="s">
+      <c r="B15" s="23"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F15" s="23"/>
+    </row>
+    <row r="16" spans="1:6" ht="12.95" customHeight="1">
       <c r="A16" s="12"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="4" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:6" ht="12.95" customHeight="1">
       <c r="A17" s="12"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="4" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F17" s="23"/>
+    </row>
+    <row r="18" spans="1:6" ht="12.95" customHeight="1">
       <c r="A18" s="12"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="4" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F18" s="23"/>
+    </row>
+    <row r="19" spans="1:6" ht="12.95" customHeight="1">
       <c r="A19" s="12"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="4" t="s">
+      <c r="B19" s="23"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F19" s="23"/>
+    </row>
+    <row r="20" spans="1:6" ht="12.95" customHeight="1">
       <c r="A20" s="12"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="4" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F20" s="23"/>
+    </row>
+    <row r="21" spans="1:6" ht="12.95" customHeight="1">
       <c r="A21" s="12"/>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F21" s="23"/>
+    </row>
+    <row r="22" spans="1:6" ht="12.95" customHeight="1">
       <c r="A22" s="12"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="4" t="s">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F22" s="23"/>
+    </row>
+    <row r="23" spans="1:6" ht="12.95" customHeight="1">
       <c r="A23" s="12"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="4" t="s">
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="24" t="s">
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="6" t="s">
         <v>64</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="24"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="21"/>
+    <row r="25" spans="1:6">
+      <c r="A25" s="10"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="24"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="21"/>
+      <c r="F25" s="23"/>
+    </row>
+    <row r="26" spans="1:6" ht="18" customHeight="1">
+      <c r="A26" s="10"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="6"/>
       <c r="E26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27" s="24"/>
-      <c r="B27" s="9" t="s">
+      <c r="F26" s="23"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="10"/>
+      <c r="B27" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="6" t="s">
         <v>65</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A28" s="24"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="21"/>
+      <c r="F27" s="23"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="10"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="6"/>
       <c r="E28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29" s="24"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="21"/>
+      <c r="F28" s="23"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="10"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="6"/>
       <c r="E29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30" s="24"/>
-      <c r="B30" s="9" t="s">
+      <c r="F29" s="23"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="10"/>
+      <c r="B30" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="6" t="s">
         <v>66</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31" s="24"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="21"/>
+      <c r="F30" s="23"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="10"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A32" s="24"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="21"/>
+      <c r="F31" s="23"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="10"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="6"/>
       <c r="E32" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="24"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="21"/>
+      <c r="F32" s="23"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="10"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="6"/>
       <c r="E33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34" s="24"/>
-      <c r="B34" s="9" t="s">
+      <c r="F33" s="23"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="10"/>
+      <c r="B34" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="24"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="21"/>
+      <c r="F34" s="23"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="10"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="6"/>
       <c r="E35" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="24"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="21"/>
+      <c r="F35" s="23"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="10"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="6"/>
       <c r="E36" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="16" t="s">
+      <c r="F36" s="24"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="15" t="s">
         <v>91</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="11" t="s">
         <v>68</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="19"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="18"/>
+    <row r="38" spans="1:6">
+      <c r="A38" s="18"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="11"/>
       <c r="E38" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39" s="19"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="18"/>
+      <c r="F38" s="23"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="18"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="11"/>
       <c r="E39" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="19"/>
+      <c r="F39" s="23"/>
+    </row>
+    <row r="40" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A40" s="18"/>
       <c r="B40" s="12" t="s">
         <v>81</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D40" s="11" t="s">
         <v>69</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F40" s="6"/>
-    </row>
-    <row r="41" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="19"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="18"/>
+      <c r="F40" s="23"/>
+    </row>
+    <row r="41" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A41" s="18"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="11"/>
       <c r="E41" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F41" s="6"/>
-    </row>
-    <row r="42" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="19"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="18"/>
+      <c r="F41" s="23"/>
+    </row>
+    <row r="42" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A42" s="18"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="11"/>
       <c r="E42" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="6"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A43" s="19"/>
+      <c r="F42" s="23"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="18"/>
       <c r="B43" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="11" t="s">
         <v>70</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44" s="19"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="18"/>
+      <c r="F43" s="23"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="18"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="11"/>
       <c r="E44" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F44" s="6"/>
-    </row>
-    <row r="45" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="19"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="18"/>
+      <c r="F44" s="23"/>
+    </row>
+    <row r="45" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A45" s="18"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="11"/>
       <c r="E45" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F45" s="6"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="19"/>
+      <c r="F45" s="23"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="18"/>
       <c r="B46" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D46" s="11" t="s">
         <v>47</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F46" s="6"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A47" s="19"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="18"/>
+      <c r="F46" s="23"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="18"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="11"/>
       <c r="E47" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F47" s="6"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A48" s="19"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="18"/>
+      <c r="F47" s="23"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="18"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="11"/>
       <c r="E48" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F48" s="6"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="19"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="18"/>
+      <c r="F48" s="23"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="18"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="11"/>
       <c r="E49" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="6"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="20"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="18"/>
+      <c r="F49" s="23"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="19"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="11"/>
       <c r="E50" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F50" s="7"/>
+      <c r="F50" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="F3:F13"/>
+    <mergeCell ref="F14:F23"/>
+    <mergeCell ref="F24:F36"/>
+    <mergeCell ref="F37:F50"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="A37:A50"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="B46:B50"/>
     <mergeCell ref="D24:D26"/>
     <mergeCell ref="D27:D29"/>
     <mergeCell ref="D30:D33"/>
@@ -2844,37 +2884,9 @@
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="A37:A50"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="F3:F13"/>
-    <mergeCell ref="F14:F23"/>
-    <mergeCell ref="F24:F36"/>
-    <mergeCell ref="F37:F50"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C30:C33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>